<commit_message>
update with cursor and add main api
</commit_message>
<xml_diff>
--- a/sample_numbers.xlsx
+++ b/sample_numbers.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,192 +436,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>9362135057</t>
+          <t>9358883639</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>9160304331</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>9362062107</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>9370317539</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>9378195071</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>9101903562</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>9368527630</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>9913037019</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9366462109</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>9126602987</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>9361175324</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>9335103716</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>9385617691</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>9940582004</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>9101287122</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>9198887977</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>John Doe</t>
+          <t>Mani agah</t>
         </is>
       </c>
     </row>

</xml_diff>